<commit_message>
explored knn and decision trees
</commit_message>
<xml_diff>
--- a/ML/knn.xlsx
+++ b/ML/knn.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Interview Prep\AI Engineer\ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B9BD3F-482A-495F-B77C-CCDAA99FAB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB00F21-9593-45FF-8754-4B01EC5D9E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10967" yWindow="0" windowWidth="11244" windowHeight="11831" xr2:uid="{6CCD3EF7-5772-4BCF-A2F6-9AE5729A2ADB}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" activeTab="1" xr2:uid="{6CCD3EF7-5772-4BCF-A2F6-9AE5729A2ADB}"/>
   </bookViews>
   <sheets>
     <sheet name="KNN" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="DT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="45">
   <si>
     <t>KNN Algorithm</t>
   </si>
@@ -112,13 +112,73 @@
   </si>
   <si>
     <t>&lt;- Predicted</t>
+  </si>
+  <si>
+    <t>Competition</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Profit/Loss</t>
+  </si>
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Mid</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up </t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Decision Tree Algorithm</t>
+  </si>
+  <si>
+    <t>Problem Statement : For a given new transaction, there will be profit/loss.</t>
+  </si>
+  <si>
+    <t>Y Variable: Profit/Loss</t>
+  </si>
+  <si>
+    <t>X Variable: Age, Type, Competition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +197,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -301,19 +369,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -323,23 +382,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -438,180 +508,6 @@
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -659,25 +555,51 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -750,29 +672,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31CB1710-DA70-44F5-878B-F3186898DBD4}" name="Table1" displayName="Table1" ref="A5:E16" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31CB1710-DA70-44F5-878B-F3186898DBD4}" name="Table1" displayName="Table1" ref="A5:E16" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="A5:E16" xr:uid="{31CB1710-DA70-44F5-878B-F3186898DBD4}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A557A252-F4AE-4AAA-A072-0A85E6161FEC}" name="Name " dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{44486262-144D-4BD3-B72D-8F2EAA2E1A70}" name="Age" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{6E00FEDE-D120-4DC4-830D-17E6CA263FDE}" name="Gender" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{1B1974AE-5618-4AB1-8733-61CC3FEFC958}" name="Gender_M" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{1D7AEEE1-AC80-4BC0-9F60-20B2EC3A5F39}" name="Game" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{A557A252-F4AE-4AAA-A072-0A85E6161FEC}" name="Name " dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{44486262-144D-4BD3-B72D-8F2EAA2E1A70}" name="Age" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{6E00FEDE-D120-4DC4-830D-17E6CA263FDE}" name="Gender" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{1B1974AE-5618-4AB1-8733-61CC3FEFC958}" name="Gender_M" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{1D7AEEE1-AC80-4BC0-9F60-20B2EC3A5F39}" name="Game" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8FFF295F-8E9A-4A4B-B56F-3758E3F2E5DA}" name="Table13" displayName="Table13" ref="A1:D12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
-  <autoFilter ref="A1:D12" xr:uid="{8FFF295F-8E9A-4A4B-B56F-3758E3F2E5DA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1969D350-F74D-46A3-91BE-B0BB3E1FB840}" name="Table3" displayName="Table3" ref="A4:D14" totalsRowShown="0">
+  <autoFilter ref="A4:D14" xr:uid="{1969D350-F74D-46A3-91BE-B0BB3E1FB840}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F0BF2422-470E-4FE9-9F05-E5FD1FBC9535}" name="Name " dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{06DD0E66-FE6B-4A13-8C52-C56B0BA9107F}" name="Age" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{0524FFF6-21CF-4987-BFB7-8E52E37A9CDA}" name="Gender" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{E299FB6F-007A-4062-BFDD-06F6570973FD}" name="Game" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{3B14CF2F-CEF2-4005-B084-0FCFAE30AD87}" name="Age"/>
+    <tableColumn id="2" xr3:uid="{58DDADAC-7123-46AD-AD55-6225AAEDA646}" name="Competition"/>
+    <tableColumn id="3" xr3:uid="{7F76CE63-8D44-4FAA-9B7A-E3BAB18B175A}" name="Type"/>
+    <tableColumn id="4" xr3:uid="{EF7D6003-2E9F-495E-90F8-015793DB2FE8}" name="Profit/Loss"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1095,7 +1017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82F27EE-68BE-48BA-8BF0-5B21FF805ED8}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="64" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -1106,313 +1028,313 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:24" ht="15.55" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="E2" s="4" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="E2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
     </row>
     <row r="3" spans="1:24" ht="15.55" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:24" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>25</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="11">
         <f>SQRT(POWER((Table1[[#This Row],[Age]]-$B$18),2)+POWER((Table1[[#This Row],[Gender_M]]-$D$18),2))</f>
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>27</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="11">
         <f>SQRT(POWER((Table1[[#This Row],[Age]]-$B$18),2)+POWER((Table1[[#This Row],[Gender_M]]-$D$18),2))</f>
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>1</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="11">
         <f>SQRT(POWER((Table1[[#This Row],[Age]]-$B$18),2)+POWER((Table1[[#This Row],[Gender_M]]-$D$18),2))</f>
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>1</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="11">
         <f>SQRT(POWER((Table1[[#This Row],[Age]]-$B$18),2)+POWER((Table1[[#This Row],[Gender_M]]-$D$18),2))</f>
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>1</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="11">
         <f>SQRT(POWER((Table1[[#This Row],[Age]]-$B$18),2)+POWER((Table1[[#This Row],[Gender_M]]-$D$18),2))</f>
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>29</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="11">
         <f>SQRT(POWER((Table1[[#This Row],[Age]]-$B$18),2)+POWER((Table1[[#This Row],[Gender_M]]-$D$18),2))</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>35</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>0</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="11">
         <f>SQRT(POWER((Table1[[#This Row],[Age]]-$B$18),2)+POWER((Table1[[#This Row],[Gender_M]]-$D$18),2))</f>
         <v>5.0990195135927845</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>18</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>0</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="11">
         <f>SQRT(POWER((Table1[[#This Row],[Age]]-$B$18),2)+POWER((Table1[[#This Row],[Gender_M]]-$D$18),2))</f>
         <v>12.041594578792296</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>21</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>0</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="11">
         <f>SQRT(POWER((Table1[[#This Row],[Age]]-$B$18),2)+POWER((Table1[[#This Row],[Gender_M]]-$D$18),2))</f>
         <v>9.0553851381374173</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>22</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>1</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="11">
         <f>SQRT(POWER((Table1[[#This Row],[Age]]-$B$18),2)+POWER((Table1[[#This Row],[Gender_M]]-$D$18),2))</f>
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="9">
         <v>31</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="9">
         <v>1</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="11">
         <f>SQRT(POWER((Table1[[#This Row],[Age]]-$B$18),2)+POWER((Table1[[#This Row],[Gender_M]]-$D$18),2))</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>30</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1422,11 +1344,9 @@
     <mergeCell ref="E2:X2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F16">
+    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="0" priority="2" percent="1" bottom="1" rank="10"/>
     <cfRule type="top10" priority="3" percent="1" bottom="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6:F16">
-    <cfRule type="top10" dxfId="0" priority="2" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1438,183 +1358,209 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CADD10-F0E6-4E7B-8847-C6D1651504D5}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.296875" customWidth="1"/>
+    <col min="4" max="4" width="10.8984375" customWidth="1"/>
+    <col min="7" max="7" width="7.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.09765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3">
-        <v>23</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="3">
-        <v>21</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="3">
-        <v>22</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="12">
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>20</v>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="E1:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>